<commit_message>
Update test case data, disable GetbearerToken entry point
</commit_message>
<xml_diff>
--- a/Test Cases/tc01_GetLibrary.xlsx
+++ b/Test Cases/tc01_GetLibrary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/darren_cheng_uipath_com/Documents/My Processes (Stormtrooper)/Synchronise Libraries/Test Cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{9C76A9DA-2011-4B30-96C9-C84D790CA42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61C26043-0D18-48D5-91D1-3571C97B4789}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{9C76A9DA-2011-4B30-96C9-C84D790CA42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DD07B06-23A1-440F-805A-EE1D7F466680}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{E9C2F1FD-B638-4B75-8C95-F261AE193CB1}"/>
+    <workbookView xWindow="5820" yWindow="5940" windowWidth="19020" windowHeight="11940" xr2:uid="{E9C2F1FD-B638-4B75-8C95-F261AE193CB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>OrchestratorHostname</t>
   </si>
@@ -59,6 +59,18 @@
   </si>
   <si>
     <t>Password$</t>
+  </si>
+  <si>
+    <t>orch2.dc.local</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Password2$</t>
+  </si>
+  <si>
+    <t>Host</t>
   </si>
 </sst>
 </file>
@@ -419,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C7975C-C739-4306-A959-DEBB36BD7E41}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,6 +473,34 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>